<commit_message>
add mac filepath compatibility
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F80355F-287E-454B-8B9E-AFEC2AA4CA9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F5663-AAF5-494F-A838-373DFAC58640}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add reset to bottom, clarify target unique names
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stanford\projects\general\PowerPoint-auto-coding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75F5663-AAF5-494F-A838-373DFAC58640}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F45E2CF-CAE9-428D-B2CA-16A3F79E0DE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38640" yWindow="10140" windowWidth="19530" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="92">
   <si>
     <t>file</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>automating file</t>
+  </si>
+  <si>
+    <t>measure11_highPerf</t>
+  </si>
+  <si>
+    <t>measure11_lowPerf</t>
   </si>
 </sst>
 </file>
@@ -790,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP11"/>
+  <dimension ref="A1:AR12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="AI10" workbookViewId="0">
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -821,12 +827,13 @@
     <col min="34" max="34" width="24.81640625" customWidth="1"/>
     <col min="35" max="35" width="24.90625" customWidth="1"/>
     <col min="36" max="36" width="26.08984375" customWidth="1"/>
-    <col min="37" max="37" width="8.7265625" style="19"/>
-    <col min="38" max="40" width="8.7265625" style="20"/>
-    <col min="41" max="41" width="8.7265625" style="21"/>
+    <col min="37" max="38" width="24.90625" customWidth="1"/>
+    <col min="39" max="39" width="8.7265625" style="19"/>
+    <col min="40" max="42" width="8.7265625" style="20"/>
+    <col min="43" max="43" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:44" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -935,26 +942,32 @@
       <c r="AJ1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AK1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="17" t="s">
+      <c r="AN1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AO1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AP1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AO1" s="18" t="s">
+      <c r="AQ1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1013,26 +1026,26 @@
       <c r="AF2" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="19">
+      <c r="AM2" s="19">
         <v>2</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AN2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AM2" s="20">
-        <v>3</v>
-      </c>
-      <c r="AN2" s="20">
+      <c r="AO2" s="20">
+        <v>3</v>
+      </c>
+      <c r="AP2" s="20">
         <v>4</v>
       </c>
-      <c r="AO2" s="21">
+      <c r="AQ2" s="21">
         <v>5</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1085,23 +1098,23 @@
       <c r="AF3" t="s">
         <v>45</v>
       </c>
-      <c r="AK3" s="19">
+      <c r="AM3" s="19">
         <v>1</v>
       </c>
-      <c r="AL3" s="20" t="s">
+      <c r="AN3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AM3" s="20">
+      <c r="AO3" s="20">
         <v>1</v>
       </c>
-      <c r="AN3" s="20">
+      <c r="AP3" s="20">
         <v>4</v>
       </c>
-      <c r="AO3" s="21">
+      <c r="AQ3" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1163,23 +1176,23 @@
       <c r="AF4" t="s">
         <v>63</v>
       </c>
-      <c r="AK4" s="19">
+      <c r="AM4" s="19">
         <v>1</v>
       </c>
-      <c r="AL4" s="20" t="s">
+      <c r="AN4" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AM4" s="20">
+      <c r="AO4" s="20">
         <v>4</v>
       </c>
-      <c r="AN4" s="20">
+      <c r="AP4" s="20">
         <v>2</v>
       </c>
-      <c r="AO4" s="21">
+      <c r="AQ4" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1256,23 +1269,23 @@
       <c r="AJ5">
         <v>2</v>
       </c>
-      <c r="AK5" s="19">
-        <v>3</v>
-      </c>
-      <c r="AL5" s="20" t="s">
+      <c r="AM5" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="AM5" s="20">
+      <c r="AO5" s="20">
         <v>4</v>
       </c>
-      <c r="AN5" s="20">
+      <c r="AP5" s="20">
         <v>2</v>
       </c>
-      <c r="AO5" s="21">
+      <c r="AQ5" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1346,23 +1359,23 @@
       <c r="AJ6">
         <v>2</v>
       </c>
-      <c r="AK6" s="19">
-        <v>3</v>
-      </c>
-      <c r="AL6" s="20" t="s">
+      <c r="AM6" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="AM6" s="20">
-        <v>3</v>
-      </c>
-      <c r="AN6" s="20">
+      <c r="AO6" s="20">
+        <v>3</v>
+      </c>
+      <c r="AP6" s="20">
         <v>2</v>
       </c>
-      <c r="AO6" s="21">
+      <c r="AQ6" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1436,23 +1449,23 @@
       <c r="AJ7">
         <v>2</v>
       </c>
-      <c r="AK7" s="19">
-        <v>3</v>
-      </c>
-      <c r="AL7" s="20" t="s">
+      <c r="AM7" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AM7" s="20">
-        <v>3</v>
-      </c>
-      <c r="AN7" s="20">
+      <c r="AO7" s="20">
+        <v>3</v>
+      </c>
+      <c r="AP7" s="20">
         <v>1</v>
       </c>
-      <c r="AO7" s="21">
+      <c r="AQ7" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1520,23 +1533,23 @@
       <c r="AJ8">
         <v>2</v>
       </c>
-      <c r="AK8" s="19">
+      <c r="AM8" s="19">
         <v>1</v>
       </c>
-      <c r="AL8" s="20" t="s">
+      <c r="AN8" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="AM8" s="20">
-        <v>3</v>
-      </c>
-      <c r="AN8" s="20">
+      <c r="AO8" s="20">
+        <v>3</v>
+      </c>
+      <c r="AP8" s="20">
         <v>4</v>
       </c>
-      <c r="AO8" s="21">
+      <c r="AQ8" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1607,23 +1620,23 @@
       <c r="AJ9">
         <v>3</v>
       </c>
-      <c r="AK9" s="19">
+      <c r="AM9" s="19">
         <v>2</v>
       </c>
-      <c r="AL9" s="20" t="s">
+      <c r="AN9" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="AM9" s="20">
+      <c r="AO9" s="20">
         <v>1</v>
       </c>
-      <c r="AN9" s="20">
-        <v>3</v>
-      </c>
-      <c r="AO9" s="21">
+      <c r="AP9" s="20">
+        <v>3</v>
+      </c>
+      <c r="AQ9" s="21">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -1694,23 +1707,23 @@
       <c r="AJ10">
         <v>1</v>
       </c>
-      <c r="AK10" s="19">
-        <v>3</v>
-      </c>
-      <c r="AL10" s="20" t="s">
+      <c r="AM10" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AM10" s="20">
+      <c r="AO10" s="20">
         <v>1</v>
       </c>
-      <c r="AN10" s="20">
+      <c r="AP10" s="20">
         <v>5</v>
       </c>
-      <c r="AO10" s="21">
+      <c r="AQ10" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1780,21 +1793,24 @@
       <c r="AJ11">
         <v>3</v>
       </c>
-      <c r="AK11" s="19">
-        <v>3</v>
-      </c>
-      <c r="AL11" s="20" t="s">
+      <c r="AM11" s="19">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AM11" s="20">
+      <c r="AO11" s="20">
         <v>4</v>
       </c>
-      <c r="AN11" s="20">
+      <c r="AP11" s="20">
         <v>2</v>
       </c>
-      <c r="AO11" s="21">
-        <v>3</v>
-      </c>
+      <c r="AQ11" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>